<commit_message>
Modificacion sobre concentrado de metricas Febrero
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150227.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150227.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Organizacional\Medicion y Monitoreo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -148,7 +148,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -225,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,12 +276,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -289,6 +283,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,9 +459,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -486,10 +492,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="96" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -539,32 +545,38 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="9" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="9" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="9" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="9" fontId="9" fillId="10" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="11" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="8" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="8" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="12" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="97">
@@ -1011,7 +1023,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1082,10 +1093,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>140</c:v>
+                  <c:v>91.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>45.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45.600000000000009</c:v>
@@ -1210,11 +1221,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1229718768"/>
-        <c:axId val="-1229723120"/>
+        <c:axId val="398937376"/>
+        <c:axId val="398936816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1229718768"/>
+        <c:axId val="398937376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1224,7 +1235,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1229723120"/>
+        <c:crossAx val="398936816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1232,7 +1243,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1229723120"/>
+        <c:axId val="398936816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,14 +1254,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1229718768"/>
+        <c:crossAx val="398937376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1359,11 +1369,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1199257280"/>
-        <c:axId val="-1199260544"/>
+        <c:axId val="288568448"/>
+        <c:axId val="288569008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1199257280"/>
+        <c:axId val="288568448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,7 +1383,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1199260544"/>
+        <c:crossAx val="288569008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1381,7 +1391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1199260544"/>
+        <c:axId val="288569008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1393,7 +1403,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1199257280"/>
+        <c:crossAx val="288568448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1513,11 +1523,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1199260000"/>
-        <c:axId val="-1199256736"/>
+        <c:axId val="288571808"/>
+        <c:axId val="291501392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1199260000"/>
+        <c:axId val="288571808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1527,7 +1537,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1199256736"/>
+        <c:crossAx val="291501392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1535,7 +1545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1199256736"/>
+        <c:axId val="291501392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1547,7 +1557,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1199260000"/>
+        <c:crossAx val="288571808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1600,7 +1610,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1709,11 +1718,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1229722032"/>
-        <c:axId val="-1229572000"/>
+        <c:axId val="104207392"/>
+        <c:axId val="104207952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1229722032"/>
+        <c:axId val="104207392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1723,7 +1732,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1229572000"/>
+        <c:crossAx val="104207952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1731,7 +1740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1229572000"/>
+        <c:axId val="104207952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1744,7 +1753,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1229722032"/>
+        <c:crossAx val="104207392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1834,10 +1843,10 @@
             <c:numRef>
               <c:f>'Desviacion de costos'!$C$20:$C$21</c:f>
               <c:numCache>
-                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11653</c:v>
+                  <c:v>9989</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5693.7300000000005</c:v>
@@ -1884,7 +1893,7 @@
             <c:numRef>
               <c:f>'Desviacion de costos'!$D$20:$D$21</c:f>
               <c:numCache>
-                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1910,11 +1919,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1229573632"/>
-        <c:axId val="-1229573088"/>
+        <c:axId val="288297600"/>
+        <c:axId val="288298160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1229573632"/>
+        <c:axId val="288297600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1924,7 +1933,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1229573088"/>
+        <c:crossAx val="288298160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1932,18 +1941,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1229573088"/>
+        <c:axId val="288298160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:numFmt formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1229573632"/>
+        <c:crossAx val="288297600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2064,11 +2073,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1229569280"/>
-        <c:axId val="-1229571456"/>
+        <c:axId val="151470032"/>
+        <c:axId val="151470592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1229569280"/>
+        <c:axId val="151470032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2078,7 +2087,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1229571456"/>
+        <c:crossAx val="151470592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2086,7 +2095,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1229571456"/>
+        <c:axId val="151470592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2099,7 +2108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1229569280"/>
+        <c:crossAx val="151470032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2210,11 +2219,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1324861936"/>
-        <c:axId val="-1324859216"/>
+        <c:axId val="151472832"/>
+        <c:axId val="151473392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1324861936"/>
+        <c:axId val="151472832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,7 +2233,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1324859216"/>
+        <c:crossAx val="151473392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2232,7 +2241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1324859216"/>
+        <c:axId val="151473392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2243,7 +2252,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1324861936"/>
+        <c:crossAx val="151472832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2360,11 +2369,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1324858672"/>
-        <c:axId val="-1328038528"/>
+        <c:axId val="104188032"/>
+        <c:axId val="104188592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1324858672"/>
+        <c:axId val="104188032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2374,7 +2383,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1328038528"/>
+        <c:crossAx val="104188592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2382,7 +2391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1328038528"/>
+        <c:axId val="104188592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2394,7 +2403,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1324858672"/>
+        <c:crossAx val="104188032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2511,11 +2520,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1445415392"/>
-        <c:axId val="-1445419200"/>
+        <c:axId val="150660384"/>
+        <c:axId val="150660944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1445415392"/>
+        <c:axId val="150660384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2525,7 +2534,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1445419200"/>
+        <c:crossAx val="150660944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2533,7 +2542,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1445419200"/>
+        <c:axId val="150660944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2545,7 +2554,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1445415392"/>
+        <c:crossAx val="150660384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2662,11 +2671,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1199263264"/>
-        <c:axId val="-1199259456"/>
+        <c:axId val="104260640"/>
+        <c:axId val="104261200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1199263264"/>
+        <c:axId val="104260640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2676,7 +2685,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1199259456"/>
+        <c:crossAx val="104261200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2684,7 +2693,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1199259456"/>
+        <c:axId val="104261200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2696,7 +2705,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1199263264"/>
+        <c:crossAx val="104260640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2813,11 +2822,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1199261632"/>
-        <c:axId val="-1199250752"/>
+        <c:axId val="293554272"/>
+        <c:axId val="293554832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1199261632"/>
+        <c:axId val="293554272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2827,7 +2836,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1199250752"/>
+        <c:crossAx val="293554832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2835,7 +2844,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1199250752"/>
+        <c:axId val="293554832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2847,7 +2856,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1199261632"/>
+        <c:crossAx val="293554272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3595,7 +3604,7 @@
   <dimension ref="A1:V88"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3645,41 +3654,41 @@
       </c>
     </row>
     <row r="20" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="42" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="32">
-        <v>140</v>
+        <v>91.2</v>
       </c>
       <c r="E20" s="32">
         <v>0</v>
       </c>
-      <c r="F20" s="39">
+      <c r="F20" s="37">
         <f>(D20-E20)/D20</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="35"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="32">
-        <v>140</v>
+        <v>45.6</v>
       </c>
       <c r="E21" s="32">
         <v>0</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="37">
         <f t="shared" ref="F21:F23" si="0">(D21-E21)/D21</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="16" t="s">
@@ -3691,13 +3700,13 @@
       <c r="E22" s="32">
         <v>25</v>
       </c>
-      <c r="F22" s="42">
+      <c r="F22" s="39">
         <f t="shared" si="0"/>
         <v>0.45175438596491241</v>
       </c>
     </row>
     <row r="23" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="35"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="16" t="s">
         <v>6</v>
       </c>
@@ -3707,7 +3716,7 @@
       <c r="E23" s="32">
         <v>80</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="40">
         <f t="shared" si="0"/>
         <v>0.12280701754385981</v>
       </c>
@@ -3739,7 +3748,7 @@
       <c r="E25" s="30">
         <v>2.4</v>
       </c>
-      <c r="F25" s="40">
+      <c r="F25" s="38">
         <f t="shared" ref="F25:F26" si="1">(D25-E25)/D25</f>
         <v>-0.19999999999999996</v>
       </c>
@@ -3755,7 +3764,7 @@
       <c r="E26" s="34">
         <v>0.17</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="38">
         <f t="shared" si="1"/>
         <v>0.65999999999999992</v>
       </c>
@@ -4249,8 +4258,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4264,7 +4273,7 @@
   <dimension ref="B1:E31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4318,12 +4327,12 @@
         <v>4</v>
       </c>
       <c r="C20" s="15">
-        <v>11653</v>
+        <v>9989</v>
       </c>
       <c r="D20" s="15">
         <v>0</v>
       </c>
-      <c r="E20" s="36">
+      <c r="E20" s="35">
         <f>(C20-D20)/C20</f>
         <v>1</v>
       </c>
@@ -4338,7 +4347,7 @@
       <c r="D21" s="15">
         <v>4685.1000000000004</v>
       </c>
-      <c r="E21" s="37">
+      <c r="E21" s="36">
         <f t="shared" ref="E21" si="0">(C21-D21)/C21</f>
         <v>0.17714749382215175</v>
       </c>
@@ -4436,7 +4445,7 @@
       <c r="F4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="43">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -4644,7 +4653,7 @@
   <dimension ref="B2:I39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D6"/>
+      <selection activeCell="G4" sqref="G4:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4702,7 +4711,7 @@
       <c r="C4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="45">
         <v>1</v>
       </c>
       <c r="E4" s="23" t="s">
@@ -4711,7 +4720,7 @@
       <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="46">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -4725,7 +4734,7 @@
       <c r="C5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="45">
         <v>1</v>
       </c>
       <c r="E5" s="23" t="s">
@@ -4734,7 +4743,7 @@
       <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="46">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -4748,7 +4757,7 @@
       <c r="C6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="45">
         <v>1</v>
       </c>
       <c r="E6" s="23" t="s">
@@ -4757,7 +4766,7 @@
       <c r="F6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="46">
         <f>AVERAGE(D6:F6)</f>
         <v>1</v>
       </c>
@@ -5060,7 +5069,7 @@
       <c r="C4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="45">
         <v>1</v>
       </c>
       <c r="E4" s="23" t="s">
@@ -5069,7 +5078,7 @@
       <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="46">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -5083,7 +5092,7 @@
       <c r="C5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="45">
         <v>1</v>
       </c>
       <c r="E5" s="23" t="s">
@@ -5092,7 +5101,7 @@
       <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="46">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -5195,7 +5204,7 @@
   <dimension ref="B2:I34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5262,7 +5271,7 @@
       <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="47">
         <f>AVERAGE(D4:F4)</f>
         <v>0.75</v>
       </c>
@@ -5276,7 +5285,7 @@
       <c r="C5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="45">
         <v>1</v>
       </c>
       <c r="E5" s="23" t="s">
@@ -5285,7 +5294,7 @@
       <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="46">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>

</xml_diff>